<commit_message>
finish BCubed calculations and export of clusters. Week 24 notes. Complete R eval pipeline
</commit_message>
<xml_diff>
--- a/Data/Scores_Full.xlsx
+++ b/Data/Scores_Full.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15200" yWindow="-19080" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="2320" yWindow="1580" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Algorithm</t>
   </si>
@@ -69,13 +69,22 @@
   </si>
   <si>
     <t>Bcubed F-Score</t>
+  </si>
+  <si>
+    <t>Rand</t>
+  </si>
+  <si>
+    <t>Adjusted Rand</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.00000000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -94,6 +103,14 @@
       <color rgb="FF000000"/>
       <name val="Helvetica"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -103,7 +120,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -111,14 +128,126 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,120 +525,315 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2">
         <v>0.18181818</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
+        <v>0.67854999999999999</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.25341000000000002</v>
+      </c>
+      <c r="E2" s="3">
         <v>0.97033898305099997</v>
       </c>
-      <c r="D2">
+      <c r="F2" s="3">
         <v>0.33961864406800002</v>
       </c>
-      <c r="E2">
+      <c r="G2" s="4">
         <v>0.50313873195199998</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>0.28571428999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="C3" s="2">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.92059999999999997</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.98305084745799998</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.86716101694900005</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.92147649573900003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="C4" s="2">
+        <v>0.95150000000000001</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.8982</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.98305084745799998</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.83665254237300002</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.90396269568300003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="C5" s="2">
+        <v>0.9667</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.93069999999999997</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.97033898305099997</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.93495762711899999</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.95231978921500005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2">
         <v>0.28571428999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="C6" s="2">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.92059999999999997</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.98305084745799998</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.86716101694900005</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.92147649573900003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="C7" s="2">
+        <v>0.9667</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.93069999999999997</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.97033898305099997</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.93495762711899999</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.95231978921500005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>0.18181818</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="C8" s="2">
+        <v>0.67854999999999999</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.25341000000000002</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.97033898305099997</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.33961864406800002</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.50313873195199998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="2">
         <v>0.28571428999999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="C9" s="2">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.92059999999999997</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.98305084745799998</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.86716101694900005</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0.92147649573900003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="5">
         <v>0</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.91579999999999995</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.82140000000000002</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.95480225988699996</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.73205205811100005</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0.82872000501999998</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B10">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C10">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D10">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E10">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F10">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
update week notes, update experiment, update thesis doc
</commit_message>
<xml_diff>
--- a/Data/Scores_Full.xlsx
+++ b/Data/Scores_Full.xlsx
@@ -226,7 +226,6 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -242,10 +241,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -528,7 +530,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -543,25 +545,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -569,22 +571,22 @@
       <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>0.18181818</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>0.67854999999999999</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>0.25341000000000002</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>0.97033898305099997</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>0.33961864406800002</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>0.50313873195199998</v>
       </c>
     </row>
@@ -592,22 +594,22 @@
       <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>0.28571428999999998</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>0.96199999999999997</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>0.92059999999999997</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>0.98305084745799998</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>0.86716101694900005</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>0.92147649573900003</v>
       </c>
     </row>
@@ -615,22 +617,22 @@
       <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>0.25</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>0.95150000000000001</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>0.8982</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.98305084745799998</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>0.83665254237300002</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>0.90396269568300003</v>
       </c>
     </row>
@@ -638,22 +640,22 @@
       <c r="A5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>0.4</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>0.9667</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>0.93069999999999997</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>0.97033898305099997</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>0.93495762711899999</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>0.95231978921500005</v>
       </c>
     </row>
@@ -661,22 +663,22 @@
       <c r="A6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>0.28571428999999998</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>0.96199999999999997</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>0.92059999999999997</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>0.98305084745799998</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>0.86716101694900005</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>0.92147649573900003</v>
       </c>
     </row>
@@ -684,22 +686,22 @@
       <c r="A7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>0.4</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>0.9667</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>0.93069999999999997</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>0.97033898305099997</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>0.93495762711899999</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>0.95231978921500005</v>
       </c>
     </row>
@@ -707,22 +709,22 @@
       <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>0.18181818</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>0.67854999999999999</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>0.25341000000000002</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>0.97033898305099997</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>0.33961864406800002</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>0.50313873195199998</v>
       </c>
     </row>
@@ -730,22 +732,22 @@
       <c r="A9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>0.28571428999999998</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>0.96199999999999997</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>0.92059999999999997</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>0.98305084745799998</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>0.86716101694900005</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>0.92147649573900003</v>
       </c>
     </row>
@@ -753,22 +755,22 @@
       <c r="A10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>0</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>0.91579999999999995</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>0.82140000000000002</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>0.95480225988699996</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>0.73205205811100005</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>0.82872000501999998</v>
       </c>
     </row>
@@ -846,5 +848,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>